<commit_message>
chore: update run artifacts and task inputs
</commit_message>
<xml_diff>
--- a/eval/responses/claude-opus-4-5-20251101/20260114_165753_squashed/h-003_output_1.xlsx
+++ b/eval/responses/claude-opus-4-5-20251101/20260114_165753_squashed/h-003_output_1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Code\ib-bench\eval\responses\claude-opus-4-5-20251101\20260114_072507\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Code\ib-bench\eval\responses\claude-opus-4-5-20251101\20260114_165753_squashed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45628D1A-4F9D-4913-961B-096A34EA730D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A9B56A-68EB-453A-B917-79142062105F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1140,8 +1140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1424,7 +1424,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>